<commit_message>
CS oumayma + BD
</commit_message>
<xml_diff>
--- a/public/listeproduit.xlsx
+++ b/public/listeproduit.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khadija\Desktop\khaled\Ecocycla\Ecocycla\public\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17071DBB-893A-4181-B606-7C30F32B4257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Produit" sheetId="1" r:id="rId4"/>
+    <sheet name="Produit" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>nomP</t>
   </si>
@@ -32,26 +37,44 @@
     <t xml:space="preserve">idcatP </t>
   </si>
   <si>
-    <t>produit1</t>
-  </si>
-  <si>
-    <t>produit 1 categorie 1</t>
-  </si>
-  <si>
-    <t>ppppppppp</t>
+    <t>Nettoyant multi-surfaces à la menthe et à l'eucalyptus</t>
+  </si>
+  <si>
+    <t>Spray de 750 ml
+Poids net 0.750000
+Référence 1333803
+CONSEILS D’UTILISATION
+Pour nettoyer et faire briller les sanitaires ( robinetterie, lavabos, carrelage) vaporiser sur la surface, laisser agir, frotter si besoin, rincer puis essuyer. Pour respecter l'environnement, suivre les dosages préconisés. Pour plus d'informations, www.biovie.com.
+COMPOSITION
+AQUA,CITRIC ACID,LACTIC ACID,CAPRYL GLUCOSIDE,AMMONIUM LAURYL SULFATE,ALCOHOL,ALCOHOL C12-18 ETHOXYLATED,SODIUM CITRATE,ORGANIC MENTHA VIRIDIS LEAF OIL,PARFUM,ISOPROPYL ALCOHOL,LIMONENE,LINALOOL,ORGANIC EUCALYPTUS GLOBULUS OIL</t>
+  </si>
+  <si>
+    <t>produit d'entretient</t>
+  </si>
+  <si>
+    <t>Savon noir liquide à l'huile de lin</t>
+  </si>
+  <si>
+    <t>Bouteille d'1L
+Poids net 1.026000
+Référence 1333080
+CONSEILS D’UTILISATION
+- Cuisine : Mettre un peu de savon noir sur une éponge. Laver et rincer à l'eau chaude.
+- Sol carrelé : Diluer 2-3 bouchons dans un seau d'eau chaude.
+- Linge :  Étaler un peu de savon noir sur la tache. Frictionner délicatement et placer en machine. Toujours faire un essai préalable. Peut être utilisé comme lessive pour linge délicat. 4 à 6 bouchons par machine.
+Précautions : provoque une sévère irritation des yeux. Tenir hors de portée des enfants. En cas de consultation d’un médecin, garder à disposition le récipient ou l’étiquette. Porter un équipement de protection des yeux, un équipement de protection du visage.
+En cas de contact avec les yeux : rincer avec précaution à l’eau pendant plusieurs minutes. Enlever les lentilles de contact si la victime en porte et si elles peuvent être facilement enlevées. Continuer à rincer.
+Si l’irritation oculaire persiste: consulter un médecin. Aérer les pièces au moins dix minutes pendant et après le nettoyage, en été comme en hiver.
+COMPOSITION
+AQUA FATTY ACIDS, C16-18 AND C18-UNSATD, POTASSIUM SALTS,POTASSIUM CARBONATE,GLYCERIN,SODIUM CITRATE,TRISODIUM SALT OF METHYL GLYCINEDIACETIC ACID,LINUM USITATISSIMUM OIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -78,13 +101,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -374,19 +405,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="49" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,35 +434,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>43.0</v>
+        <v>7.8</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>4.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>